<commit_message>
Signed-off-by: zied99 <ziedici@gmail.Com>Les différentes critéres à mesurer dans l'application Signed-off-by: zied99 <ziedici@gmail.Com>Fiche de mesure de la qualité logiciel Signed-off-by: zied99 <ziedici@gmail.Com>
</commit_message>
<xml_diff>
--- a/Gestion de projet/PAQL/Fonctionalités/Exploitabilité.xlsx
+++ b/Gestion de projet/PAQL/Fonctionalités/Exploitabilité.xlsx
@@ -161,9 +161,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -182,6 +179,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,7 +591,7 @@
   <dimension ref="A2:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,89 +603,77 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>3</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>4</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="C9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>